<commit_message>
fixed up project1 blt and bgt confusion. added enw bits for project2
</commit_message>
<xml_diff>
--- a/projects/cs2200-project-1/microcode.xlsx
+++ b/projects/cs2200-project-1/microcode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruh\Documents\GT\Fall 2023\CS_2200\projects\cs2200-project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA2FDF9-87A0-489F-B994-7ABB4855684C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3C354C-ECB9-464D-97CD-EB278F16726F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -729,6 +729,8 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -777,13 +779,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF5050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1059,8 +1073,8 @@
   <dimension ref="A1:AP997"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O36" sqref="O36"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P55" sqref="P55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
@@ -1091,14 +1105,14 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
       <c r="I1" s="3" t="s">
         <v>3</v>
       </c>
@@ -2046,7 +2060,7 @@
       <c r="AD10" s="4"/>
       <c r="AE10" s="4"/>
       <c r="AF10" s="7" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(     BIN2HEX(_xlfn.CONCAT(AC10, AB10),1),     BIN2HEX(_xlfn.CONCAT(AA10,Z10,Y10, X10),1),     BIN2HEX(_xlfn.CONCAT(W10,V10,U10, T10),1),     BIN2HEX(_xlfn.CONCAT(S10,R10,Q10, P10),1),     BIN2HEX(_xlfn.CONCAT(O10,N10, M10, L10),1),     BIN2HEX(_xlfn.CONCAT(K10,J10,C10,D10),1),     BIN2HEX(_xlfn.CONCAT(E10,F10,G10,H10),1) )</f>
         <v>0840100</v>
       </c>
     </row>
@@ -3435,7 +3449,7 @@
         <v>0</v>
       </c>
       <c r="I25" s="5">
-        <f t="shared" ref="I25:I45" si="4">BIN2DEC(_xlfn.CONCAT(C25:H25))</f>
+        <f t="shared" ref="I25:I40" si="4">BIN2DEC(_xlfn.CONCAT(C25:H25))</f>
         <v>0</v>
       </c>
       <c r="J25" s="2">
@@ -3501,7 +3515,7 @@
       <c r="AD25" s="4"/>
       <c r="AE25" s="4"/>
       <c r="AF25" s="7" t="str">
-        <f t="shared" ref="AF25:AF45" si="5">_xlfn.CONCAT(     BIN2HEX(_xlfn.CONCAT(AC25, AB25),1),     BIN2HEX(_xlfn.CONCAT(AA25,Z25,Y25, X25),1),     BIN2HEX(_xlfn.CONCAT(W25,V25,U25, T25),1),     BIN2HEX(_xlfn.CONCAT(S25,R25,Q25, P25),1),     BIN2HEX(_xlfn.CONCAT(O25,N25, M25, L25),1),     BIN2HEX(_xlfn.CONCAT(K25,J25,C25,D25),1),     BIN2HEX(_xlfn.CONCAT(E25,F25,G25,H25),1) )</f>
+        <f t="shared" ref="AF25:AF40" si="5">_xlfn.CONCAT(     BIN2HEX(_xlfn.CONCAT(AC25, AB25),1),     BIN2HEX(_xlfn.CONCAT(AA25,Z25,Y25, X25),1),     BIN2HEX(_xlfn.CONCAT(W25,V25,U25, T25),1),     BIN2HEX(_xlfn.CONCAT(S25,R25,Q25, P25),1),     BIN2HEX(_xlfn.CONCAT(O25,N25, M25, L25),1),     BIN2HEX(_xlfn.CONCAT(K25,J25,C25,D25),1),     BIN2HEX(_xlfn.CONCAT(E25,F25,G25,H25),1) )</f>
         <v>2000000</v>
       </c>
     </row>
@@ -4145,10 +4159,10 @@
         <v>0</v>
       </c>
       <c r="S32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T32" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U32" s="2">
         <v>0</v>
@@ -4181,7 +4195,7 @@
       <c r="AE32" s="4"/>
       <c r="AF32" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>001005F</v>
+        <v>000805F</v>
       </c>
     </row>
     <row r="33" spans="1:33" ht="14.25" customHeight="1">
@@ -4242,10 +4256,10 @@
         <v>0</v>
       </c>
       <c r="S33" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U33" s="2">
         <v>0</v>
@@ -4278,10 +4292,10 @@
       <c r="AE33" s="4"/>
       <c r="AF33" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>0108060</v>
+        <v>0110060</v>
       </c>
     </row>
-    <row r="34" spans="1:33" s="41" customFormat="1" ht="14.25" customHeight="1">
+    <row r="34" spans="1:33" s="25" customFormat="1" ht="14.25" customHeight="1">
       <c r="A34" s="4">
         <f t="shared" si="3"/>
         <v>32</v>
@@ -4373,7 +4387,7 @@
       </c>
       <c r="AD34" s="4"/>
       <c r="AE34" s="4"/>
-      <c r="AF34" s="40" t="str">
+      <c r="AF34" s="24" t="str">
         <f t="shared" si="5"/>
         <v>0420121</v>
       </c>
@@ -4824,10 +4838,10 @@
         <v>0</v>
       </c>
       <c r="S39" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T39" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U39" s="2">
         <v>0</v>
@@ -4860,7 +4874,7 @@
       <c r="AE39" s="4"/>
       <c r="AF39" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>0008066</v>
+        <v>0010066</v>
       </c>
       <c r="AG39" s="4" t="s">
         <v>21</v>
@@ -4924,10 +4938,10 @@
         <v>0</v>
       </c>
       <c r="S40" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T40" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U40" s="2">
         <v>0</v>
@@ -4960,39 +4974,41 @@
       <c r="AE40" s="4"/>
       <c r="AF40" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>0110060</v>
+        <v>0108060</v>
       </c>
     </row>
-    <row r="41" spans="1:33" s="41" customFormat="1" ht="14.25" customHeight="1">
+    <row r="41" spans="1:33" s="25" customFormat="1" ht="14.25" customHeight="1">
       <c r="A41" s="4">
         <f t="shared" si="3"/>
         <v>39</v>
       </c>
-      <c r="B41" s="2"/>
+      <c r="B41" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="C41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D41" s="2">
         <v>0</v>
       </c>
       <c r="E41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F41" s="2">
         <v>0</v>
       </c>
       <c r="G41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41" s="2">
         <v>0</v>
       </c>
       <c r="I41" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f>BIN2DEC(_xlfn.CONCAT(C41:H41))</f>
+        <v>42</v>
       </c>
       <c r="J41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41" s="2">
         <v>0</v>
@@ -5019,7 +5035,7 @@
         <v>0</v>
       </c>
       <c r="S41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T41" s="2">
         <v>0</v>
@@ -5034,7 +5050,7 @@
         <v>0</v>
       </c>
       <c r="X41" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y41" s="2">
         <v>0</v>
@@ -5048,14 +5064,14 @@
       <c r="AB41" s="2">
         <v>0</v>
       </c>
-      <c r="AC41" s="2">
+      <c r="AC41" s="23">
         <v>0</v>
       </c>
       <c r="AD41" s="4"/>
       <c r="AE41" s="4"/>
-      <c r="AF41" s="40" t="str">
-        <f t="shared" si="5"/>
-        <v>0000000</v>
+      <c r="AF41" s="24" t="str">
+        <f>_xlfn.CONCAT(     BIN2HEX(_xlfn.CONCAT(AC41, AB41),1),     BIN2HEX(_xlfn.CONCAT(AA41,Z41,Y41, X41),1),     BIN2HEX(_xlfn.CONCAT(W41,V41,U41, T41),1),     BIN2HEX(_xlfn.CONCAT(S41,R41,Q41, P41),1),     BIN2HEX(_xlfn.CONCAT(O41,N41, M41, L41),1),     BIN2HEX(_xlfn.CONCAT(K41,J41,C41,D41),1),     BIN2HEX(_xlfn.CONCAT(E41,F41,G41,H41),1) )</f>
+        <v>010806A</v>
       </c>
     </row>
     <row r="42" spans="1:33" ht="14.25" customHeight="1">
@@ -5063,31 +5079,33 @@
         <f t="shared" si="3"/>
         <v>40</v>
       </c>
-      <c r="B42" s="2"/>
+      <c r="B42" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="C42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D42" s="2">
         <v>0</v>
       </c>
       <c r="E42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F42" s="2">
         <v>0</v>
       </c>
       <c r="G42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f>BIN2DEC(_xlfn.CONCAT(C42:H42))</f>
+        <v>43</v>
       </c>
       <c r="J42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" s="2">
         <v>0</v>
@@ -5117,7 +5135,7 @@
         <v>0</v>
       </c>
       <c r="T42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U42" s="2">
         <v>0</v>
@@ -5132,7 +5150,7 @@
         <v>0</v>
       </c>
       <c r="Y42" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z42" s="2">
         <v>0</v>
@@ -5143,14 +5161,14 @@
       <c r="AB42" s="2">
         <v>0</v>
       </c>
-      <c r="AC42" s="2">
+      <c r="AC42" s="23">
         <v>0</v>
       </c>
       <c r="AD42" s="4"/>
       <c r="AE42" s="4"/>
       <c r="AF42" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>0000000</v>
+        <f>_xlfn.CONCAT(     BIN2HEX(_xlfn.CONCAT(AC42, AB42),1),     BIN2HEX(_xlfn.CONCAT(AA42,Z42,Y42, X42),1),     BIN2HEX(_xlfn.CONCAT(W42,V42,U42, T42),1),     BIN2HEX(_xlfn.CONCAT(S42,R42,Q42, P42),1),     BIN2HEX(_xlfn.CONCAT(O42,N42, M42, L42),1),     BIN2HEX(_xlfn.CONCAT(K42,J42,C42,D42),1),     BIN2HEX(_xlfn.CONCAT(E42,F42,G42,H42),1) )</f>
+        <v>021006B</v>
       </c>
     </row>
     <row r="43" spans="1:33" ht="14.25" customHeight="1">
@@ -5159,32 +5177,32 @@
         <v>41</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D43" s="2">
         <v>0</v>
       </c>
       <c r="E43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F43" s="2">
         <v>0</v>
       </c>
       <c r="G43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H43" s="2">
         <v>0</v>
       </c>
       <c r="I43" s="5">
-        <f t="shared" si="4"/>
-        <v>42</v>
+        <f>BIN2DEC(_xlfn.CONCAT(C43:H43))</f>
+        <v>0</v>
       </c>
       <c r="J43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K43" s="2">
         <v>0</v>
@@ -5193,7 +5211,7 @@
         <v>0</v>
       </c>
       <c r="M43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N43" s="2">
         <v>0</v>
@@ -5211,7 +5229,7 @@
         <v>0</v>
       </c>
       <c r="S43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T43" s="2">
         <v>0</v>
@@ -5220,13 +5238,13 @@
         <v>0</v>
       </c>
       <c r="V43" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W43" s="2">
         <v>0</v>
       </c>
       <c r="X43" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y43" s="2">
         <v>0</v>
@@ -5246,8 +5264,8 @@
       <c r="AD43" s="4"/>
       <c r="AE43" s="4"/>
       <c r="AF43" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>010806A</v>
+        <f>_xlfn.CONCAT(     BIN2HEX(_xlfn.CONCAT(AC43, AB43),1),     BIN2HEX(_xlfn.CONCAT(AA43,Z43,Y43, X43),1),     BIN2HEX(_xlfn.CONCAT(W43,V43,U43, T43),1),     BIN2HEX(_xlfn.CONCAT(S43,R43,Q43, P43),1),     BIN2HEX(_xlfn.CONCAT(O43,N43, M43, L43),1),     BIN2HEX(_xlfn.CONCAT(K43,J43,C43,D43),1),     BIN2HEX(_xlfn.CONCAT(E43,F43,G43,H43),1) )</f>
+        <v>0040200</v>
       </c>
     </row>
     <row r="44" spans="1:33" ht="14.25" customHeight="1">
@@ -5255,96 +5273,93 @@
         <f t="shared" si="3"/>
         <v>42</v>
       </c>
-      <c r="B44" s="2" t="s">
-        <v>102</v>
-      </c>
       <c r="C44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D44" s="2">
         <v>0</v>
       </c>
       <c r="E44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F44" s="2">
         <v>0</v>
       </c>
       <c r="G44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" s="5">
-        <f t="shared" si="4"/>
-        <v>43</v>
-      </c>
-      <c r="J44" s="2">
-        <v>1</v>
-      </c>
-      <c r="K44" s="2">
-        <v>0</v>
-      </c>
-      <c r="L44" s="2">
-        <v>0</v>
-      </c>
-      <c r="M44" s="2">
-        <v>0</v>
-      </c>
-      <c r="N44" s="2">
-        <v>0</v>
-      </c>
-      <c r="O44" s="2">
-        <v>0</v>
-      </c>
-      <c r="P44" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q44" s="2">
-        <v>0</v>
-      </c>
-      <c r="R44" s="2">
-        <v>0</v>
-      </c>
-      <c r="S44" s="2">
-        <v>0</v>
-      </c>
-      <c r="T44" s="2">
-        <v>1</v>
-      </c>
-      <c r="U44" s="2">
-        <v>0</v>
-      </c>
-      <c r="V44" s="2">
-        <v>0</v>
-      </c>
-      <c r="W44" s="2">
-        <v>0</v>
-      </c>
-      <c r="X44" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y44" s="2">
-        <v>1</v>
-      </c>
-      <c r="Z44" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA44" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB44" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC44" s="23">
+        <f>BIN2DEC(_xlfn.CONCAT(C44:H44))</f>
+        <v>0</v>
+      </c>
+      <c r="J44" s="19">
+        <v>0</v>
+      </c>
+      <c r="K44" s="19">
+        <v>0</v>
+      </c>
+      <c r="L44" s="19">
+        <v>0</v>
+      </c>
+      <c r="M44" s="19">
+        <v>0</v>
+      </c>
+      <c r="N44" s="19">
+        <v>0</v>
+      </c>
+      <c r="O44" s="19">
+        <v>0</v>
+      </c>
+      <c r="P44" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="19">
+        <v>0</v>
+      </c>
+      <c r="R44" s="19">
+        <v>0</v>
+      </c>
+      <c r="S44" s="19">
+        <v>0</v>
+      </c>
+      <c r="T44" s="19">
+        <v>0</v>
+      </c>
+      <c r="U44" s="19">
+        <v>0</v>
+      </c>
+      <c r="V44" s="19">
+        <v>0</v>
+      </c>
+      <c r="W44" s="19">
+        <v>0</v>
+      </c>
+      <c r="X44" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB44" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC44" s="19">
         <v>0</v>
       </c>
       <c r="AD44" s="4"/>
       <c r="AE44" s="4"/>
       <c r="AF44" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>021006B</v>
+        <f>_xlfn.CONCAT(     BIN2HEX(_xlfn.CONCAT(AC44, AB44),1),     BIN2HEX(_xlfn.CONCAT(AA44,Z44,Y44, X44),1),     BIN2HEX(_xlfn.CONCAT(W44,V44,U44, T44),1),     BIN2HEX(_xlfn.CONCAT(S44,R44,Q44, P44),1),     BIN2HEX(_xlfn.CONCAT(O44,N44, M44, L44),1),     BIN2HEX(_xlfn.CONCAT(K44,J44,C44,D44),1),     BIN2HEX(_xlfn.CONCAT(E44,F44,G44,H44),1) )</f>
+        <v>0000000</v>
       </c>
     </row>
     <row r="45" spans="1:33" ht="14.25" customHeight="1">
@@ -5352,9 +5367,6 @@
         <f t="shared" si="3"/>
         <v>43</v>
       </c>
-      <c r="B45" s="2" t="s">
-        <v>103</v>
-      </c>
       <c r="C45" s="2">
         <v>0</v>
       </c>
@@ -5374,74 +5386,74 @@
         <v>0</v>
       </c>
       <c r="I45" s="5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="J45" s="2">
-        <v>0</v>
-      </c>
-      <c r="K45" s="2">
-        <v>0</v>
-      </c>
-      <c r="L45" s="2">
-        <v>0</v>
-      </c>
-      <c r="M45" s="2">
-        <v>1</v>
-      </c>
-      <c r="N45" s="2">
-        <v>0</v>
-      </c>
-      <c r="O45" s="2">
-        <v>0</v>
-      </c>
-      <c r="P45" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q45" s="2">
-        <v>0</v>
-      </c>
-      <c r="R45" s="2">
-        <v>0</v>
-      </c>
-      <c r="S45" s="2">
-        <v>0</v>
-      </c>
-      <c r="T45" s="2">
-        <v>0</v>
-      </c>
-      <c r="U45" s="2">
-        <v>0</v>
-      </c>
-      <c r="V45" s="2">
-        <v>1</v>
-      </c>
-      <c r="W45" s="2">
-        <v>0</v>
-      </c>
-      <c r="X45" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y45" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB45" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC45" s="23">
+        <f>BIN2DEC(_xlfn.CONCAT(C45:H45))</f>
+        <v>0</v>
+      </c>
+      <c r="J45" s="19">
+        <v>0</v>
+      </c>
+      <c r="K45" s="19">
+        <v>0</v>
+      </c>
+      <c r="L45" s="19">
+        <v>0</v>
+      </c>
+      <c r="M45" s="19">
+        <v>0</v>
+      </c>
+      <c r="N45" s="19">
+        <v>0</v>
+      </c>
+      <c r="O45" s="19">
+        <v>0</v>
+      </c>
+      <c r="P45" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="19">
+        <v>0</v>
+      </c>
+      <c r="R45" s="19">
+        <v>0</v>
+      </c>
+      <c r="S45" s="19">
+        <v>0</v>
+      </c>
+      <c r="T45" s="19">
+        <v>0</v>
+      </c>
+      <c r="U45" s="19">
+        <v>0</v>
+      </c>
+      <c r="V45" s="19">
+        <v>0</v>
+      </c>
+      <c r="W45" s="19">
+        <v>0</v>
+      </c>
+      <c r="X45" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z45" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA45" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB45" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="19">
         <v>0</v>
       </c>
       <c r="AD45" s="4"/>
       <c r="AE45" s="4"/>
       <c r="AF45" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>0040200</v>
+        <f>_xlfn.CONCAT(     BIN2HEX(_xlfn.CONCAT(AC45, AB45),1),     BIN2HEX(_xlfn.CONCAT(AA45,Z45,Y45, X45),1),     BIN2HEX(_xlfn.CONCAT(W45,V45,U45, T45),1),     BIN2HEX(_xlfn.CONCAT(S45,R45,Q45, P45),1),     BIN2HEX(_xlfn.CONCAT(O45,N45, M45, L45),1),     BIN2HEX(_xlfn.CONCAT(K45,J45,C45,D45),1),     BIN2HEX(_xlfn.CONCAT(E45,F45,G45,H45),1) )</f>
+        <v>0000000</v>
       </c>
     </row>
     <row r="46" spans="1:33" ht="14.25" customHeight="1">
@@ -5472,64 +5484,64 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J46" s="2">
-        <v>0</v>
-      </c>
-      <c r="K46" s="2">
-        <v>0</v>
-      </c>
-      <c r="L46" s="2">
-        <v>0</v>
-      </c>
-      <c r="M46" s="2">
-        <v>0</v>
-      </c>
-      <c r="N46" s="2">
-        <v>0</v>
-      </c>
-      <c r="O46" s="2">
-        <v>0</v>
-      </c>
-      <c r="P46" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q46" s="2">
-        <v>0</v>
-      </c>
-      <c r="R46" s="2">
-        <v>0</v>
-      </c>
-      <c r="S46" s="2">
-        <v>0</v>
-      </c>
-      <c r="T46" s="2">
-        <v>0</v>
-      </c>
-      <c r="U46" s="2">
-        <v>0</v>
-      </c>
-      <c r="V46" s="2">
-        <v>0</v>
-      </c>
-      <c r="W46" s="2">
-        <v>0</v>
-      </c>
-      <c r="X46" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y46" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB46" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC46" s="2">
+      <c r="J46" s="19">
+        <v>0</v>
+      </c>
+      <c r="K46" s="19">
+        <v>0</v>
+      </c>
+      <c r="L46" s="19">
+        <v>0</v>
+      </c>
+      <c r="M46" s="19">
+        <v>0</v>
+      </c>
+      <c r="N46" s="19">
+        <v>0</v>
+      </c>
+      <c r="O46" s="19">
+        <v>0</v>
+      </c>
+      <c r="P46" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="19">
+        <v>0</v>
+      </c>
+      <c r="R46" s="19">
+        <v>0</v>
+      </c>
+      <c r="S46" s="19">
+        <v>0</v>
+      </c>
+      <c r="T46" s="19">
+        <v>0</v>
+      </c>
+      <c r="U46" s="19">
+        <v>0</v>
+      </c>
+      <c r="V46" s="19">
+        <v>0</v>
+      </c>
+      <c r="W46" s="19">
+        <v>0</v>
+      </c>
+      <c r="X46" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA46" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB46" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC46" s="19">
         <v>0</v>
       </c>
       <c r="AD46" s="4"/>
@@ -5567,64 +5579,64 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J47" s="2">
-        <v>0</v>
-      </c>
-      <c r="K47" s="2">
-        <v>0</v>
-      </c>
-      <c r="L47" s="2">
-        <v>0</v>
-      </c>
-      <c r="M47" s="2">
-        <v>0</v>
-      </c>
-      <c r="N47" s="2">
-        <v>0</v>
-      </c>
-      <c r="O47" s="2">
-        <v>0</v>
-      </c>
-      <c r="P47" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q47" s="2">
-        <v>0</v>
-      </c>
-      <c r="R47" s="2">
-        <v>0</v>
-      </c>
-      <c r="S47" s="2">
-        <v>0</v>
-      </c>
-      <c r="T47" s="2">
-        <v>0</v>
-      </c>
-      <c r="U47" s="2">
-        <v>0</v>
-      </c>
-      <c r="V47" s="2">
-        <v>0</v>
-      </c>
-      <c r="W47" s="2">
-        <v>0</v>
-      </c>
-      <c r="X47" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y47" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z47" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA47" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB47" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC47" s="2">
+      <c r="J47" s="19">
+        <v>0</v>
+      </c>
+      <c r="K47" s="19">
+        <v>0</v>
+      </c>
+      <c r="L47" s="19">
+        <v>0</v>
+      </c>
+      <c r="M47" s="19">
+        <v>0</v>
+      </c>
+      <c r="N47" s="19">
+        <v>0</v>
+      </c>
+      <c r="O47" s="19">
+        <v>0</v>
+      </c>
+      <c r="P47" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="19">
+        <v>0</v>
+      </c>
+      <c r="R47" s="19">
+        <v>0</v>
+      </c>
+      <c r="S47" s="19">
+        <v>0</v>
+      </c>
+      <c r="T47" s="19">
+        <v>0</v>
+      </c>
+      <c r="U47" s="19">
+        <v>0</v>
+      </c>
+      <c r="V47" s="19">
+        <v>0</v>
+      </c>
+      <c r="W47" s="19">
+        <v>0</v>
+      </c>
+      <c r="X47" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB47" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC47" s="19">
         <v>0</v>
       </c>
       <c r="AD47" s="4"/>
@@ -5662,64 +5674,64 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J48" s="2">
-        <v>0</v>
-      </c>
-      <c r="K48" s="2">
-        <v>0</v>
-      </c>
-      <c r="L48" s="2">
-        <v>0</v>
-      </c>
-      <c r="M48" s="2">
-        <v>0</v>
-      </c>
-      <c r="N48" s="2">
-        <v>0</v>
-      </c>
-      <c r="O48" s="2">
-        <v>0</v>
-      </c>
-      <c r="P48" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q48" s="2">
-        <v>0</v>
-      </c>
-      <c r="R48" s="2">
-        <v>0</v>
-      </c>
-      <c r="S48" s="2">
-        <v>0</v>
-      </c>
-      <c r="T48" s="2">
-        <v>0</v>
-      </c>
-      <c r="U48" s="2">
-        <v>0</v>
-      </c>
-      <c r="V48" s="2">
-        <v>0</v>
-      </c>
-      <c r="W48" s="2">
-        <v>0</v>
-      </c>
-      <c r="X48" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y48" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z48" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA48" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB48" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC48" s="2">
+      <c r="J48" s="19">
+        <v>0</v>
+      </c>
+      <c r="K48" s="19">
+        <v>0</v>
+      </c>
+      <c r="L48" s="19">
+        <v>0</v>
+      </c>
+      <c r="M48" s="19">
+        <v>0</v>
+      </c>
+      <c r="N48" s="19">
+        <v>0</v>
+      </c>
+      <c r="O48" s="19">
+        <v>0</v>
+      </c>
+      <c r="P48" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="19">
+        <v>0</v>
+      </c>
+      <c r="R48" s="19">
+        <v>0</v>
+      </c>
+      <c r="S48" s="19">
+        <v>0</v>
+      </c>
+      <c r="T48" s="19">
+        <v>0</v>
+      </c>
+      <c r="U48" s="19">
+        <v>0</v>
+      </c>
+      <c r="V48" s="19">
+        <v>0</v>
+      </c>
+      <c r="W48" s="19">
+        <v>0</v>
+      </c>
+      <c r="X48" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y48" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA48" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB48" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC48" s="19">
         <v>0</v>
       </c>
       <c r="AD48" s="4"/>
@@ -5760,61 +5772,61 @@
       <c r="J49" s="19">
         <v>0</v>
       </c>
-      <c r="K49" s="2">
-        <v>0</v>
-      </c>
-      <c r="L49" s="2">
-        <v>0</v>
-      </c>
-      <c r="M49" s="2">
-        <v>0</v>
-      </c>
-      <c r="N49" s="2">
-        <v>0</v>
-      </c>
-      <c r="O49" s="2">
-        <v>0</v>
-      </c>
-      <c r="P49" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q49" s="2">
-        <v>0</v>
-      </c>
-      <c r="R49" s="2">
-        <v>0</v>
-      </c>
-      <c r="S49" s="2">
-        <v>0</v>
-      </c>
-      <c r="T49" s="2">
-        <v>0</v>
-      </c>
-      <c r="U49" s="2">
-        <v>0</v>
-      </c>
-      <c r="V49" s="2">
-        <v>0</v>
-      </c>
-      <c r="W49" s="2">
-        <v>0</v>
-      </c>
-      <c r="X49" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y49" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z49" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA49" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB49" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC49" s="2">
+      <c r="K49" s="19">
+        <v>0</v>
+      </c>
+      <c r="L49" s="19">
+        <v>0</v>
+      </c>
+      <c r="M49" s="19">
+        <v>0</v>
+      </c>
+      <c r="N49" s="19">
+        <v>0</v>
+      </c>
+      <c r="O49" s="19">
+        <v>0</v>
+      </c>
+      <c r="P49" s="19">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="19">
+        <v>0</v>
+      </c>
+      <c r="R49" s="19">
+        <v>0</v>
+      </c>
+      <c r="S49" s="19">
+        <v>0</v>
+      </c>
+      <c r="T49" s="19">
+        <v>0</v>
+      </c>
+      <c r="U49" s="19">
+        <v>0</v>
+      </c>
+      <c r="V49" s="19">
+        <v>0</v>
+      </c>
+      <c r="W49" s="19">
+        <v>0</v>
+      </c>
+      <c r="X49" s="19">
+        <v>0</v>
+      </c>
+      <c r="Y49" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z49" s="19">
+        <v>0</v>
+      </c>
+      <c r="AA49" s="19">
+        <v>0</v>
+      </c>
+      <c r="AB49" s="19">
+        <v>0</v>
+      </c>
+      <c r="AC49" s="19">
         <v>0</v>
       </c>
       <c r="AD49" s="4"/>
@@ -5833,30 +5845,30 @@
       <c r="AE52" s="4"/>
     </row>
     <row r="53" spans="1:40" ht="14.25" customHeight="1">
-      <c r="B53" s="34" t="s">
+      <c r="B53" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="C53" s="34"/>
-      <c r="D53" s="34"/>
-      <c r="E53" s="34"/>
-      <c r="F53" s="34"/>
-      <c r="G53" s="34"/>
-      <c r="H53" s="34"/>
-      <c r="I53" s="34"/>
-      <c r="J53" s="34"/>
-      <c r="M53" s="37" t="s">
+      <c r="C53" s="36"/>
+      <c r="D53" s="36"/>
+      <c r="E53" s="36"/>
+      <c r="F53" s="36"/>
+      <c r="G53" s="36"/>
+      <c r="H53" s="36"/>
+      <c r="I53" s="36"/>
+      <c r="J53" s="36"/>
+      <c r="M53" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="N53" s="38"/>
-      <c r="O53" s="38"/>
-      <c r="P53" s="39"/>
-      <c r="R53" s="31" t="s">
+      <c r="N53" s="40"/>
+      <c r="O53" s="40"/>
+      <c r="P53" s="41"/>
+      <c r="R53" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="S53" s="31"/>
-      <c r="T53" s="31"/>
-      <c r="U53" s="31"/>
-      <c r="V53" s="31"/>
+      <c r="S53" s="33"/>
+      <c r="T53" s="33"/>
+      <c r="U53" s="33"/>
+      <c r="V53" s="33"/>
       <c r="W53" s="8"/>
       <c r="X53" s="8"/>
       <c r="Y53" s="8"/>
@@ -5880,14 +5892,14 @@
       <c r="B54" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C54" s="35" t="s">
+      <c r="C54" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="35"/>
-      <c r="G54" s="35"/>
-      <c r="H54" s="35"/>
+      <c r="D54" s="37"/>
+      <c r="E54" s="37"/>
+      <c r="F54" s="37"/>
+      <c r="G54" s="37"/>
+      <c r="H54" s="37"/>
       <c r="I54" s="1" t="s">
         <v>20</v>
       </c>
@@ -5906,11 +5918,11 @@
       <c r="P54" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="R54" s="31"/>
-      <c r="S54" s="31"/>
-      <c r="T54" s="31"/>
-      <c r="U54" s="31"/>
-      <c r="V54" s="31"/>
+      <c r="R54" s="33"/>
+      <c r="S54" s="33"/>
+      <c r="T54" s="33"/>
+      <c r="U54" s="33"/>
+      <c r="V54" s="33"/>
       <c r="W54" s="8"/>
       <c r="X54" s="8"/>
       <c r="Y54" s="8"/>
@@ -5934,14 +5946,14 @@
       <c r="B55" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="C55" s="36" t="s">
+      <c r="C55" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="D55" s="36"/>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="36"/>
-      <c r="H55" s="36"/>
+      <c r="D55" s="38"/>
+      <c r="E55" s="38"/>
+      <c r="F55" s="38"/>
+      <c r="G55" s="38"/>
+      <c r="H55" s="38"/>
       <c r="I55" s="2"/>
       <c r="J55" s="11" t="str">
         <f>DEC2HEX(C55)</f>
@@ -5960,11 +5972,11 @@
         <f t="shared" ref="P55:P70" si="6">DEC2HEX(O55,2)</f>
         <v>03</v>
       </c>
-      <c r="R55" s="31"/>
-      <c r="S55" s="31"/>
-      <c r="T55" s="31"/>
-      <c r="U55" s="31"/>
-      <c r="V55" s="31"/>
+      <c r="R55" s="33"/>
+      <c r="S55" s="33"/>
+      <c r="T55" s="33"/>
+      <c r="U55" s="33"/>
+      <c r="V55" s="33"/>
       <c r="W55" s="8"/>
       <c r="X55" s="8"/>
       <c r="Y55" s="8"/>
@@ -5988,14 +6000,14 @@
       <c r="B56" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="C56" s="30" t="s">
+      <c r="C56" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
-      <c r="F56" s="30"/>
-      <c r="G56" s="30"/>
-      <c r="H56" s="30"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
       <c r="I56" s="14"/>
       <c r="J56" s="15" t="str">
         <f>DEC2HEX(C56)</f>
@@ -6014,11 +6026,11 @@
         <f t="shared" si="6"/>
         <v>06</v>
       </c>
-      <c r="R56" s="31"/>
-      <c r="S56" s="31"/>
-      <c r="T56" s="31"/>
-      <c r="U56" s="31"/>
-      <c r="V56" s="31"/>
+      <c r="R56" s="33"/>
+      <c r="S56" s="33"/>
+      <c r="T56" s="33"/>
+      <c r="U56" s="33"/>
+      <c r="V56" s="33"/>
       <c r="W56" s="8"/>
       <c r="X56" s="8"/>
       <c r="Y56" s="8"/>
@@ -6052,11 +6064,11 @@
         <f t="shared" si="6"/>
         <v>09</v>
       </c>
-      <c r="R57" s="31"/>
-      <c r="S57" s="31"/>
-      <c r="T57" s="31"/>
-      <c r="U57" s="31"/>
-      <c r="V57" s="31"/>
+      <c r="R57" s="33"/>
+      <c r="S57" s="33"/>
+      <c r="T57" s="33"/>
+      <c r="U57" s="33"/>
+      <c r="V57" s="33"/>
       <c r="AH57" s="2"/>
       <c r="AI57" s="2"/>
       <c r="AJ57" s="2"/>
@@ -6076,11 +6088,11 @@
         <f t="shared" si="6"/>
         <v>0C</v>
       </c>
-      <c r="R58" s="31"/>
-      <c r="S58" s="31"/>
-      <c r="T58" s="31"/>
-      <c r="U58" s="31"/>
-      <c r="V58" s="31"/>
+      <c r="R58" s="33"/>
+      <c r="S58" s="33"/>
+      <c r="T58" s="33"/>
+      <c r="U58" s="33"/>
+      <c r="V58" s="33"/>
       <c r="AI58" s="2"/>
       <c r="AJ58" s="2"/>
       <c r="AK58" s="2"/>
@@ -6115,13 +6127,13 @@
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="R60" s="32" t="s">
+      <c r="R60" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="S60" s="32"/>
-      <c r="T60" s="32"/>
-      <c r="U60" s="32"/>
-      <c r="V60" s="32"/>
+      <c r="S60" s="34"/>
+      <c r="T60" s="34"/>
+      <c r="U60" s="34"/>
+      <c r="V60" s="34"/>
     </row>
     <row r="61" spans="1:40" ht="14.25" customHeight="1">
       <c r="M61" s="12" t="s">
@@ -6137,11 +6149,11 @@
         <f t="shared" si="6"/>
         <v>1B</v>
       </c>
-      <c r="R61" s="32"/>
-      <c r="S61" s="32"/>
-      <c r="T61" s="32"/>
-      <c r="U61" s="32"/>
-      <c r="V61" s="32"/>
+      <c r="R61" s="34"/>
+      <c r="S61" s="34"/>
+      <c r="T61" s="34"/>
+      <c r="U61" s="34"/>
+      <c r="V61" s="34"/>
     </row>
     <row r="62" spans="1:40" ht="15" customHeight="1">
       <c r="M62" s="12" t="s">
@@ -6157,11 +6169,11 @@
         <f t="shared" si="6"/>
         <v>1D</v>
       </c>
-      <c r="R62" s="32"/>
-      <c r="S62" s="32"/>
-      <c r="T62" s="32"/>
-      <c r="U62" s="32"/>
-      <c r="V62" s="32"/>
+      <c r="R62" s="34"/>
+      <c r="S62" s="34"/>
+      <c r="T62" s="34"/>
+      <c r="U62" s="34"/>
+      <c r="V62" s="34"/>
     </row>
     <row r="63" spans="1:40" ht="14.25" customHeight="1">
       <c r="M63" s="12" t="s">
@@ -6177,11 +6189,11 @@
         <f t="shared" si="6"/>
         <v>1E</v>
       </c>
-      <c r="R63" s="32"/>
-      <c r="S63" s="32"/>
-      <c r="T63" s="32"/>
-      <c r="U63" s="32"/>
-      <c r="V63" s="32"/>
+      <c r="R63" s="34"/>
+      <c r="S63" s="34"/>
+      <c r="T63" s="34"/>
+      <c r="U63" s="34"/>
+      <c r="V63" s="34"/>
     </row>
     <row r="64" spans="1:40" ht="14.25" customHeight="1">
       <c r="M64" s="12" t="s">
@@ -6197,11 +6209,11 @@
         <f t="shared" si="6"/>
         <v>22</v>
       </c>
-      <c r="R64" s="32"/>
-      <c r="S64" s="32"/>
-      <c r="T64" s="32"/>
-      <c r="U64" s="32"/>
-      <c r="V64" s="32"/>
+      <c r="R64" s="34"/>
+      <c r="S64" s="34"/>
+      <c r="T64" s="34"/>
+      <c r="U64" s="34"/>
+      <c r="V64" s="34"/>
     </row>
     <row r="65" spans="13:42" ht="14.25" customHeight="1">
       <c r="M65" s="12" t="s">
@@ -6217,11 +6229,11 @@
         <f t="shared" si="6"/>
         <v>25</v>
       </c>
-      <c r="R65" s="32"/>
-      <c r="S65" s="32"/>
-      <c r="T65" s="32"/>
-      <c r="U65" s="32"/>
-      <c r="V65" s="32"/>
+      <c r="R65" s="34"/>
+      <c r="S65" s="34"/>
+      <c r="T65" s="34"/>
+      <c r="U65" s="34"/>
+      <c r="V65" s="34"/>
     </row>
     <row r="66" spans="13:42" ht="14.25" customHeight="1">
       <c r="M66" s="12" t="s">
@@ -6231,11 +6243,11 @@
         <v>56</v>
       </c>
       <c r="O66" s="4">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P66" s="11" t="str">
         <f t="shared" si="6"/>
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="67" spans="13:42" ht="14.25" customHeight="1">
@@ -6246,11 +6258,11 @@
         <v>56</v>
       </c>
       <c r="O67" s="4">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="P67" s="11" t="str">
         <f t="shared" si="6"/>
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="68" spans="13:42" ht="14.25" customHeight="1">
@@ -6282,19 +6294,19 @@
       <c r="P71" s="16"/>
     </row>
     <row r="72" spans="13:42" ht="14.25" customHeight="1">
-      <c r="M72" s="24" t="s">
+      <c r="M72" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="N72" s="25"/>
-      <c r="O72" s="25"/>
-      <c r="P72" s="26"/>
+      <c r="N72" s="27"/>
+      <c r="O72" s="27"/>
+      <c r="P72" s="28"/>
       <c r="AP72" s="2"/>
     </row>
     <row r="73" spans="13:42" ht="14.25" customHeight="1">
-      <c r="M73" s="27"/>
-      <c r="N73" s="28"/>
-      <c r="O73" s="28"/>
-      <c r="P73" s="29"/>
+      <c r="M73" s="29"/>
+      <c r="N73" s="30"/>
+      <c r="O73" s="30"/>
+      <c r="P73" s="31"/>
     </row>
     <row r="74" spans="13:42" ht="14.25" customHeight="1"/>
     <row r="75" spans="13:42" ht="14.25" customHeight="1"/>
@@ -7234,34 +7246,42 @@
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="C2:H49">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J43:AB48">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+  <conditionalFormatting sqref="J41:AB43">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:AC42">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AC45:AC48 J49:AC49">
-    <cfRule type="cellIs" dxfId="1" priority="11" operator="equal">
+  <conditionalFormatting sqref="J44:AC49">
+    <cfRule type="cellIs" dxfId="3" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="14" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AC43">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>